<commit_message>
Update with last figures of the paper
</commit_message>
<xml_diff>
--- a/Paper_horizon_length/Graphics/horizon_explenation.xlsx
+++ b/Paper_horizon_length/Graphics/horizon_explenation.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\Nextcloud\Github\annex71_st2_common_exercices\Use of penalized()\Graphics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerar\Nextcloud\Github\annex71_st2_common_exercices\Paper_horizon_length\Graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0649C000-DC76-4CF7-AC8E-C4FDA4A74FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A549526D-03EE-4159-A1FD-5DE1D7AB0446}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="25320" windowHeight="9150" activeTab="1" xr2:uid="{F4087B5A-F52F-4FE7-85E2-EECA0BDB5024}"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="25320" windowHeight="9150" activeTab="1" xr2:uid="{F4087B5A-F52F-4FE7-85E2-EECA0BDB5024}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="For presentation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
   <si>
     <t>MPC execution 1</t>
   </si>
@@ -180,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -196,16 +197,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -657,15 +661,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>35719</xdr:colOff>
+      <xdr:colOff>10654</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>5953</xdr:rowOff>
+      <xdr:rowOff>15979</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>255984</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>15041</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>15478</xdr:rowOff>
+      <xdr:rowOff>25504</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -680,8 +684,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3769519" y="767953"/>
-          <a:ext cx="1163240" cy="390525"/>
+          <a:off x="4021180" y="777979"/>
+          <a:ext cx="1528387" cy="390525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -710,8 +714,8 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="2400" b="1"/>
-            <a:t>horizon</a:t>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>horizon (TH)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -779,14 +783,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>141684</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>29765</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>90237</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>166689</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15039</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -801,8 +805,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3868340" y="2887265"/>
-          <a:ext cx="1602583" cy="303609"/>
+          <a:off x="4152210" y="2757237"/>
+          <a:ext cx="1930005" cy="686802"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -830,11 +834,55 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="2000" b="1"/>
             <a:t>time step</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>t</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" baseline="-25000">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2000" b="1" baseline="-25000"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -902,13 +950,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>536122</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>123312</xdr:rowOff>
+      <xdr:rowOff>123311</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>125186</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>174172</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15038</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -923,8 +971,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2364922" y="2409312"/>
-          <a:ext cx="998764" cy="812860"/>
+          <a:off x="2370938" y="2409311"/>
+          <a:ext cx="1002774" cy="1034727"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -952,10 +1000,902 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1800" b="1"/>
             <a:t>control horizon</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>(t</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="-25000"/>
+            <a:t>c</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1701</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>115303</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>5013</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>115303</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B430F0B5-EE72-4EB3-BA95-4313E822EC7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2488227" y="4471737"/>
+          <a:ext cx="2289312" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>10654</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>15979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>15041</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>25504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9008D023-8D25-4545-90CB-37C69D6291E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4011154" y="777979"/>
+          <a:ext cx="1528387" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>horizon (TH)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1610</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>101203</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>101203</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5CF32A5-208D-4BDA-A6F4-DC7E3A1572E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4764110" y="2768203"/>
+          <a:ext cx="760390" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>181788</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>90237</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>206793</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>15039</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46519937-1C42-4858-8296-39457146A191}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4192314" y="5970671"/>
+          <a:ext cx="1930005" cy="686802"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>time step</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>t</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" baseline="-25000">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2000" b="1" baseline="-25000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>37613</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>370114</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E99E298D-680E-4EBB-A0E4-9514A343031D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476013" y="2481943"/>
+          <a:ext cx="751601" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>536122</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>123311</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>125186</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>15038</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48853779-041B-4967-8E8C-6821A29F850D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2364922" y="2409311"/>
+          <a:ext cx="998764" cy="1034727"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>control horizon</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>(t</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="-25000"/>
+            <a:t>c</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1701</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>125329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>365961</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>130971</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A45698C1-81D1-4066-9EDA-1AFC7E164F6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2488227" y="887329"/>
+          <a:ext cx="2269260" cy="5642"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>146015</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>150402</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>25504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8619A895-B9C1-48C9-973E-C3CF6A37F7D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3013541" y="396979"/>
+          <a:ext cx="1528387" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>horizon (TH)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1610</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>101203</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>101203</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3668E63E-8A0D-4DFC-935B-12BC94AA31DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4774136" y="6006703"/>
+          <a:ext cx="760390" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>141684</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>90237</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>166689</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>15039</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B3F49CB-0421-44AA-9FFB-14187841F828}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4152210" y="5995737"/>
+          <a:ext cx="1930005" cy="686802"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>time step</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>t</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" baseline="-25000">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2000" b="1" baseline="-25000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2521</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>65169</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>65169</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5934230A-2E37-4EDF-A946-99160A37D21D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2489047" y="1398669"/>
+          <a:ext cx="2283479" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>115018</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>135355</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>110290</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180472</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38B2F94D-848E-4E84-886E-211341960097}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2601544" y="1468855"/>
+          <a:ext cx="1900272" cy="616617"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>control horizon</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="80000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>(t</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1" baseline="-25000"/>
+            <a:t>c</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1264,7 +2204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846717EB-8A09-44DC-A3D5-13DB2123A8CD}">
   <dimension ref="B3:AC30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="AD17" sqref="AD17"/>
     </sheetView>
   </sheetViews>
@@ -1396,11 +2336,11 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="1"/>
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
@@ -1428,9 +2368,9 @@
       <c r="AC7" s="1"/>
     </row>
     <row r="8" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="1"/>
       <c r="F8" s="6"/>
       <c r="G8" s="9"/>
@@ -1458,9 +2398,9 @@
       <c r="AC8" s="1"/>
     </row>
     <row r="9" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
       <c r="G9" s="9"/>
@@ -1488,9 +2428,9 @@
       <c r="AC9" s="1"/>
     </row>
     <row r="10" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="1"/>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
@@ -1548,11 +2488,11 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2"/>
       <c r="G12" s="5"/>
@@ -1580,9 +2520,9 @@
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
       <c r="G13" s="5"/>
@@ -1610,9 +2550,9 @@
       <c r="AC13" s="1"/>
     </row>
     <row r="14" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="4"/>
       <c r="F14" s="2"/>
       <c r="G14" s="5"/>
@@ -1640,9 +2580,9 @@
       <c r="AC14" s="1"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2"/>
       <c r="G15" s="5"/>
@@ -1700,11 +2640,11 @@
       <c r="AC16" s="1"/>
     </row>
     <row r="17" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="1"/>
       <c r="F17" s="2"/>
       <c r="G17" s="5"/>
@@ -1732,9 +2672,9 @@
       <c r="AC17" s="1"/>
     </row>
     <row r="18" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2"/>
       <c r="G18" s="5"/>
@@ -1762,9 +2702,9 @@
       <c r="AC18" s="1"/>
     </row>
     <row r="19" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="4"/>
       <c r="F19" s="2"/>
       <c r="G19" s="5"/>
@@ -1792,9 +2732,9 @@
       <c r="AC19" s="1"/>
     </row>
     <row r="20" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2"/>
       <c r="G20" s="5"/>
@@ -1822,10 +2762,10 @@
       <c r="AC20" s="1"/>
     </row>
     <row r="21" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
       <c r="G21" s="5"/>
@@ -1854,8 +2794,8 @@
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
       <c r="G22" s="5"/>
@@ -1884,8 +2824,8 @@
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
       <c r="G23" s="5"/>
@@ -1914,8 +2854,8 @@
     </row>
     <row r="24" spans="2:29" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
       <c r="E24" s="1"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
@@ -2005,12 +2945,12 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-      <c r="N26" s="14" t="s">
+      <c r="N26" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
@@ -2120,6 +3060,10 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="S25:T25"/>
     <mergeCell ref="B12:D15"/>
     <mergeCell ref="B7:D10"/>
     <mergeCell ref="B17:D20"/>
@@ -2131,10 +3075,6 @@
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="Q25:R25"/>
     <mergeCell ref="C21:D24"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="S25:T25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2145,8 +3085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0EA563-FED8-4CCF-A4A6-F3F97EF5F19F}">
   <dimension ref="B3:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2278,11 +3218,11 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="1"/>
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
@@ -2310,9 +3250,9 @@
       <c r="AC7" s="1"/>
     </row>
     <row r="8" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="1"/>
       <c r="F8" s="6"/>
       <c r="G8" s="9"/>
@@ -2340,9 +3280,9 @@
       <c r="AC8" s="1"/>
     </row>
     <row r="9" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
       <c r="G9" s="9"/>
@@ -2370,9 +3310,9 @@
       <c r="AC9" s="1"/>
     </row>
     <row r="10" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="1"/>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
@@ -2430,11 +3370,11 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2"/>
       <c r="G12" s="5"/>
@@ -2462,9 +3402,9 @@
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
       <c r="G13" s="5"/>
@@ -2492,9 +3432,9 @@
       <c r="AC13" s="1"/>
     </row>
     <row r="14" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="4"/>
       <c r="F14" s="2"/>
       <c r="G14" s="5"/>
@@ -2522,9 +3462,9 @@
       <c r="AC14" s="1"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2"/>
       <c r="G15" s="5"/>
@@ -2552,10 +3492,10 @@
       <c r="AC15" s="1"/>
     </row>
     <row r="16" spans="2:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2"/>
       <c r="G16" s="5"/>
@@ -2584,8 +3524,8 @@
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="1"/>
       <c r="F17" s="2"/>
       <c r="G17" s="5"/>
@@ -2614,8 +3554,8 @@
     </row>
     <row r="18" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2"/>
       <c r="G18" s="5"/>
@@ -2644,8 +3584,8 @@
     </row>
     <row r="19" spans="2:29" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="1"/>
       <c r="F19" s="3"/>
       <c r="G19" s="4"/>
@@ -2727,12 +3667,12 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="14" t="s">
+      <c r="L21" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
@@ -2844,17 +3784,999 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
     <mergeCell ref="S20:T20"/>
     <mergeCell ref="B7:D10"/>
     <mergeCell ref="B12:D15"/>
     <mergeCell ref="C16:D19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="I20:J20"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:R20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1923C5-6123-4774-98E6-A33333FEA1A3}">
+  <dimension ref="B3:V42"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:AW1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="0.5703125" customWidth="1"/>
+    <col min="6" max="22" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+    </row>
+    <row r="6" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+    </row>
+    <row r="8" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+    </row>
+    <row r="10" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+    </row>
+    <row r="11" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+    </row>
+    <row r="12" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+    </row>
+    <row r="13" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="2:22" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="2:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="15">
+        <v>1</v>
+      </c>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15">
+        <v>2</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15">
+        <v>3</v>
+      </c>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15">
+        <v>4</v>
+      </c>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15">
+        <v>5</v>
+      </c>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15">
+        <v>6</v>
+      </c>
+      <c r="R18" s="15"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="2:22" ht="21" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+    </row>
+    <row r="26" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+    </row>
+    <row r="29" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+    </row>
+    <row r="30" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+    </row>
+    <row r="31" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+    </row>
+    <row r="33" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="16"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B34" s="12"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B35" s="12"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+    </row>
+    <row r="36" spans="2:22" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="12"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+    </row>
+    <row r="37" spans="2:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="15">
+        <v>1</v>
+      </c>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15">
+        <v>2</v>
+      </c>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15">
+        <v>3</v>
+      </c>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15">
+        <v>4</v>
+      </c>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15">
+        <v>5</v>
+      </c>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15">
+        <v>6</v>
+      </c>
+      <c r="R37" s="15"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+    </row>
+    <row r="38" spans="2:22" ht="21" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="B24:D27"/>
+    <mergeCell ref="B29:D32"/>
+    <mergeCell ref="C33:D36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="B5:D8"/>
+    <mergeCell ref="B10:D13"/>
+    <mergeCell ref="C14:D17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K38:N38"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="K37:L37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>